<commit_message>
New script to visualize and analyze change in network density over sucessive emigrations.
</commit_message>
<xml_diff>
--- a/data/colony_sna_metrics.xlsx
+++ b/data/colony_sna_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jy33\OneDrive\Desktop\R\ant_sna\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0D6716-434F-4E7C-B7E7-8C1734423C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D0E029-1794-4DE9-A4CB-3FB96C0A825B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{C014F821-1412-4917-9742-99384016B187}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>